<commit_message>
style (mock-forecast.xlsx): rename mpcs sheet to mpc
</commit_message>
<xml_diff>
--- a/mock-forecast.xlsx
+++ b/mock-forecast.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoja\fim-shiny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625F85EB-3881-4FA3-B83E-14C494583288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C6C652-3F15-4B83-9F5C-AB81AA672ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{D8625C4B-9966-4F50-99EA-54E4F74CFE15}"/>
+    <workbookView xWindow="920" yWindow="2510" windowWidth="21640" windowHeight="11290" activeTab="1" xr2:uid="{D8625C4B-9966-4F50-99EA-54E4F74CFE15}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="mpcs" sheetId="2" r:id="rId2"/>
+    <sheet name="mpc" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -231,9 +231,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -271,7 +271,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -377,7 +377,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -519,7 +519,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -529,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{296D78E7-6801-4808-9FDF-BF8AD86C6DE2}">
   <dimension ref="B2:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -708,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7E92E2F-DB40-4B0E-9023-FFF1EA018B0C}">
   <dimension ref="B2:O101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
data(mock-forecast, mock-historical): adjust names to purchases taxes transfers
</commit_message>
<xml_diff>
--- a/mock-forecast.xlsx
+++ b/mock-forecast.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoja\fim-shiny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C6C652-3F15-4B83-9F5C-AB81AA672ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBC35B1-7789-410C-B535-559A72950FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="2510" windowWidth="21640" windowHeight="11290" activeTab="1" xr2:uid="{D8625C4B-9966-4F50-99EA-54E4F74CFE15}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D8625C4B-9966-4F50-99EA-54E4F74CFE15}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -37,21 +37,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Type of disbursement</t>
-  </si>
-  <si>
-    <t>Disbursement 1</t>
-  </si>
-  <si>
-    <t>Disbursement 2</t>
-  </si>
-  <si>
-    <t>Disbursement 3</t>
-  </si>
-  <si>
-    <t>Disbursement 4</t>
   </si>
   <si>
     <t>Total</t>
@@ -85,6 +73,15 @@
   </si>
   <si>
     <t>2026 Q1</t>
+  </si>
+  <si>
+    <t>Purchases</t>
+  </si>
+  <si>
+    <t>Taxes</t>
+  </si>
+  <si>
+    <t>Transfers</t>
   </si>
 </sst>
 </file>
@@ -527,52 +524,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{296D78E7-6801-4808-9FDF-BF8AD86C6DE2}">
-  <dimension ref="B2:K6"/>
+  <dimension ref="B2:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.08984375" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>1</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -602,9 +599,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>50</v>
@@ -634,9 +631,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>300</v>
@@ -664,38 +661,6 @@
       </c>
       <c r="K5">
         <v>380</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>36</v>
-      </c>
-      <c r="D6">
-        <v>37</v>
-      </c>
-      <c r="E6">
-        <v>37</v>
-      </c>
-      <c r="F6">
-        <v>37</v>
-      </c>
-      <c r="G6">
-        <v>36</v>
-      </c>
-      <c r="H6">
-        <v>35</v>
-      </c>
-      <c r="I6">
-        <v>34</v>
-      </c>
-      <c r="J6">
-        <v>33</v>
-      </c>
-      <c r="K6">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -709,15 +674,15 @@
   <dimension ref="B2:O101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.08984375" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -758,13 +723,13 @@
         <v>12</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="str">
         <f>data!B3</f>
-        <v>Disbursement 1</v>
+        <v>Purchases</v>
       </c>
       <c r="C3">
         <v>0.5</v>
@@ -795,10 +760,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="str">
         <f>data!B4</f>
-        <v>Disbursement 2</v>
+        <v>Taxes</v>
       </c>
       <c r="C4">
         <v>0.1</v>
@@ -835,60 +800,57 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="str">
         <f>data!B5</f>
-        <v>Disbursement 3</v>
+        <v>Transfers</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0.3</v>
+      </c>
+      <c r="D5">
+        <v>0.2</v>
+      </c>
+      <c r="E5">
+        <v>0.1</v>
+      </c>
+      <c r="F5">
+        <v>0.05</v>
+      </c>
+      <c r="G5">
+        <v>0.05</v>
+      </c>
+      <c r="H5">
+        <v>0.02</v>
+      </c>
+      <c r="I5">
+        <v>0.02</v>
+      </c>
+      <c r="J5">
+        <v>0.02</v>
+      </c>
+      <c r="K5">
+        <v>0.02</v>
+      </c>
+      <c r="L5">
+        <v>0.02</v>
       </c>
       <c r="O5" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B6" s="6" t="str">
+        <f>SUM(C5:N5)</f>
+        <v>0.80000000000000016</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
         <f>data!B6</f>
-        <v>Disbursement 4</v>
-      </c>
-      <c r="C6">
-        <v>0.3</v>
-      </c>
-      <c r="D6">
-        <v>0.2</v>
-      </c>
-      <c r="E6">
-        <v>0.1</v>
-      </c>
-      <c r="F6">
-        <v>0.05</v>
-      </c>
-      <c r="G6">
-        <v>0.05</v>
-      </c>
-      <c r="H6">
-        <v>0.02</v>
-      </c>
-      <c r="I6">
-        <v>0.02</v>
-      </c>
-      <c r="J6">
-        <v>0.02</v>
-      </c>
-      <c r="K6">
-        <v>0.02</v>
-      </c>
-      <c r="L6">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="O6" s="2">
         <f t="shared" si="0"/>
-        <v>0.80000000000000016</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="6">
         <f>data!B7</f>
         <v>0</v>
@@ -898,7 +860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="6">
         <f>data!B8</f>
         <v>0</v>
@@ -908,7 +870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
         <f>data!B9</f>
         <v>0</v>
@@ -918,7 +880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
         <f>data!B10</f>
         <v>0</v>
@@ -928,7 +890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <f>data!B11</f>
         <v>0</v>
@@ -938,7 +900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <f>data!B12</f>
         <v>0</v>
@@ -948,7 +910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <f>data!B13</f>
         <v>0</v>
@@ -958,7 +920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <f>data!B14</f>
         <v>0</v>
@@ -968,7 +930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="6">
         <f>data!B15</f>
         <v>0</v>
@@ -978,7 +940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="6">
         <f>data!B16</f>
         <v>0</v>
@@ -988,7 +950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="6">
         <f>data!B17</f>
         <v>0</v>
@@ -998,7 +960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="6">
         <f>data!B18</f>
         <v>0</v>
@@ -1008,7 +970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="6">
         <f>data!B19</f>
         <v>0</v>
@@ -1018,7 +980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="6">
         <f>data!B20</f>
         <v>0</v>
@@ -1028,7 +990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="6">
         <f>data!B21</f>
         <v>0</v>
@@ -1038,7 +1000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="6">
         <f>data!B22</f>
         <v>0</v>
@@ -1048,7 +1010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="6">
         <f>data!B23</f>
         <v>0</v>
@@ -1058,7 +1020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="6">
         <f>data!B24</f>
         <v>0</v>
@@ -1068,7 +1030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="6">
         <f>data!B25</f>
         <v>0</v>
@@ -1078,7 +1040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="6">
         <f>data!B26</f>
         <v>0</v>
@@ -1088,7 +1050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="6">
         <f>data!B27</f>
         <v>0</v>
@@ -1098,7 +1060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28" s="6">
         <f>data!B28</f>
         <v>0</v>
@@ -1108,7 +1070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29" s="6">
         <f>data!B29</f>
         <v>0</v>
@@ -1118,7 +1080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30" s="6">
         <f>data!B30</f>
         <v>0</v>
@@ -1128,7 +1090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" s="6">
         <f>data!B31</f>
         <v>0</v>
@@ -1138,7 +1100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B32" s="6">
         <f>data!B32</f>
         <v>0</v>
@@ -1148,7 +1110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" s="6">
         <f>data!B33</f>
         <v>0</v>
@@ -1158,7 +1120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34" s="6">
         <f>data!B34</f>
         <v>0</v>
@@ -1168,7 +1130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B35" s="6">
         <f>data!B35</f>
         <v>0</v>
@@ -1178,7 +1140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" s="6">
         <f>data!B36</f>
         <v>0</v>
@@ -1188,7 +1150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B37" s="6">
         <f>data!B37</f>
         <v>0</v>
@@ -1198,7 +1160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B38" s="6">
         <f>data!B38</f>
         <v>0</v>
@@ -1208,7 +1170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39" s="6">
         <f>data!B39</f>
         <v>0</v>
@@ -1218,7 +1180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B40" s="6">
         <f>data!B40</f>
         <v>0</v>
@@ -1228,7 +1190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B41" s="6">
         <f>data!B41</f>
         <v>0</v>
@@ -1238,7 +1200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42" s="6">
         <f>data!B42</f>
         <v>0</v>
@@ -1248,7 +1210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B43" s="6">
         <f>data!B43</f>
         <v>0</v>
@@ -1258,7 +1220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="6">
         <f>data!B44</f>
         <v>0</v>
@@ -1268,7 +1230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="6">
         <f>data!B45</f>
         <v>0</v>
@@ -1278,7 +1240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="6">
         <f>data!B46</f>
         <v>0</v>
@@ -1288,7 +1250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="6">
         <f>data!B47</f>
         <v>0</v>
@@ -1298,7 +1260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="6">
         <f>data!B48</f>
         <v>0</v>
@@ -1308,7 +1270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B49" s="6">
         <f>data!B49</f>
         <v>0</v>
@@ -1318,7 +1280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B50" s="6">
         <f>data!B50</f>
         <v>0</v>
@@ -1328,7 +1290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B51" s="6">
         <f>data!B51</f>
         <v>0</v>
@@ -1338,7 +1300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B52" s="6">
         <f>data!B52</f>
         <v>0</v>
@@ -1348,7 +1310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" s="6">
         <f>data!B53</f>
         <v>0</v>
@@ -1358,7 +1320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B54" s="6">
         <f>data!B54</f>
         <v>0</v>
@@ -1368,7 +1330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" s="6">
         <f>data!B55</f>
         <v>0</v>
@@ -1378,7 +1340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B56" s="6">
         <f>data!B56</f>
         <v>0</v>
@@ -1388,7 +1350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B57" s="6">
         <f>data!B57</f>
         <v>0</v>
@@ -1398,7 +1360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B58" s="6">
         <f>data!B58</f>
         <v>0</v>
@@ -1408,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B59" s="6">
         <f>data!B59</f>
         <v>0</v>
@@ -1418,7 +1380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B60" s="6">
         <f>data!B60</f>
         <v>0</v>
@@ -1428,7 +1390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B61" s="6">
         <f>data!B61</f>
         <v>0</v>
@@ -1438,7 +1400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B62" s="6">
         <f>data!B62</f>
         <v>0</v>
@@ -1448,7 +1410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B63" s="6">
         <f>data!B63</f>
         <v>0</v>
@@ -1458,7 +1420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B64" s="6">
         <f>data!B64</f>
         <v>0</v>
@@ -1468,7 +1430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B65" s="6">
         <f>data!B65</f>
         <v>0</v>
@@ -1478,7 +1440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B66" s="6">
         <f>data!B66</f>
         <v>0</v>
@@ -1488,7 +1450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B67" s="6">
         <f>data!B67</f>
         <v>0</v>
@@ -1498,7 +1460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B68" s="6">
         <f>data!B68</f>
         <v>0</v>
@@ -1508,7 +1470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B69" s="6">
         <f>data!B69</f>
         <v>0</v>
@@ -1518,7 +1480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B70" s="6">
         <f>data!B70</f>
         <v>0</v>
@@ -1528,7 +1490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B71" s="6">
         <f>data!B71</f>
         <v>0</v>
@@ -1538,7 +1500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B72" s="6">
         <f>data!B72</f>
         <v>0</v>
@@ -1548,7 +1510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B73" s="6">
         <f>data!B73</f>
         <v>0</v>
@@ -1558,7 +1520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B74" s="6">
         <f>data!B74</f>
         <v>0</v>
@@ -1568,7 +1530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B75" s="6">
         <f>data!B75</f>
         <v>0</v>
@@ -1578,7 +1540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B76" s="6">
         <f>data!B76</f>
         <v>0</v>
@@ -1588,7 +1550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B77" s="6">
         <f>data!B77</f>
         <v>0</v>
@@ -1598,7 +1560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B78" s="6">
         <f>data!B78</f>
         <v>0</v>
@@ -1608,7 +1570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B79" s="6">
         <f>data!B79</f>
         <v>0</v>
@@ -1618,7 +1580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B80" s="6">
         <f>data!B80</f>
         <v>0</v>
@@ -1628,7 +1590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B81" s="6">
         <f>data!B81</f>
         <v>0</v>
@@ -1638,7 +1600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B82" s="6">
         <f>data!B82</f>
         <v>0</v>
@@ -1648,7 +1610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B83" s="6">
         <f>data!B83</f>
         <v>0</v>
@@ -1658,7 +1620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B84" s="6">
         <f>data!B84</f>
         <v>0</v>
@@ -1668,7 +1630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B85" s="6">
         <f>data!B85</f>
         <v>0</v>
@@ -1678,7 +1640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B86" s="6">
         <f>data!B86</f>
         <v>0</v>
@@ -1688,7 +1650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B87" s="6">
         <f>data!B87</f>
         <v>0</v>
@@ -1698,7 +1660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B88" s="6">
         <f>data!B88</f>
         <v>0</v>
@@ -1708,7 +1670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B89" s="6">
         <f>data!B89</f>
         <v>0</v>
@@ -1718,7 +1680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B90" s="6">
         <f>data!B90</f>
         <v>0</v>
@@ -1728,7 +1690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B91" s="6">
         <f>data!B91</f>
         <v>0</v>
@@ -1738,7 +1700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B92" s="6">
         <f>data!B92</f>
         <v>0</v>
@@ -1748,7 +1710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B93" s="6">
         <f>data!B93</f>
         <v>0</v>
@@ -1758,7 +1720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B94" s="6">
         <f>data!B94</f>
         <v>0</v>
@@ -1768,7 +1730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B95" s="6">
         <f>data!B95</f>
         <v>0</v>
@@ -1778,7 +1740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B96" s="6">
         <f>data!B96</f>
         <v>0</v>
@@ -1788,7 +1750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B97" s="6">
         <f>data!B97</f>
         <v>0</v>
@@ -1798,7 +1760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B98" s="6">
         <f>data!B98</f>
         <v>0</v>
@@ -1808,7 +1770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B99" s="6">
         <f>data!B99</f>
         <v>0</v>
@@ -1818,7 +1780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B100" s="7">
         <f>data!B100</f>
         <v>0</v>
@@ -1840,9 +1802,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>